<commit_message>
updates and issues by sandeep
</commit_message>
<xml_diff>
--- a/routes/uploads/Exported_data.xlsx
+++ b/routes/uploads/Exported_data.xlsx
@@ -14,7 +14,245 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79" count="79">
+  <x:si>
+    <x:t>name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nature</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shares</x:t>
+  </x:si>
+  <x:si>
+    <x:t>block</x:t>
+  </x:si>
+  <x:si>
+    <x:t>floor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>unit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>estateName</x:t>
+  </x:si>
+  <x:si>
+    <x:t>account</x:t>
+  </x:si>
+  <x:si>
+    <x:t>password</x:t>
+  </x:si>
+  <x:si>
+    <x:t>admin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4uje8j7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Renae Brotherheed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SingleOwner</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gbraxhf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kearney Vero, Peter Lau</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JointOwner</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2o6e2tr</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Elysha Verheijden</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4A</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>to6x2ft</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nissa Boyle</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bz3hsdz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Keen Brimilcombe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rz7csro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Berkley Braywood</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>xcgxvth</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Forester Burrass</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>haelpq3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Donielle Blackbourn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>qx8l30q</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Windy Narup</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>918bfl0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sharlene Anespie</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2aj6dg6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Murdoch Tarply</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fprw5c3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Grills</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CorporateOwner</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fnbgach</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jodi Downs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rogxq80</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pascal Hiland</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園14</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5muqd30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Budd Fynes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>n23eqzi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lida Nesey</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>km8ub18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Edgardo Terrazzo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2zpx4at</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Menard Burditt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yke2192</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marriot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rpzy1m8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kenyon Wesson</x:t>
+  </x:si>
+  <x:si>
+    <x:t>寶翠園20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a0vaxxb</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,7 +613,644 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:0"/>
+    <x:row r="1" spans="1:9">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:9">
+      <x:c r="A2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:9">
+      <x:c r="A3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
+        <x:v>0.24</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:9">
+      <x:c r="A4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>0.56</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:9">
+      <x:c r="A5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="n">
+        <x:v>0.9</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:9">
+      <x:c r="A6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="n">
+        <x:v>0.99</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:9">
+      <x:c r="A7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="n">
+        <x:v>0.15</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="n">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:9">
+      <x:c r="A8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="n">
+        <x:v>0.18</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:9">
+      <x:c r="A9" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="n">
+        <x:v>0.26</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:9">
+      <x:c r="A10" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="n">
+        <x:v>0.65</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:9">
+      <x:c r="A11" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="n">
+        <x:v>0.8</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:9">
+      <x:c r="A12" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="n">
+        <x:v>0.29</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:9">
+      <x:c r="A13" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="n">
+        <x:v>0.41</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:9">
+      <x:c r="A14" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="n">
+        <x:v>0.11</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:9">
+      <x:c r="A15" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="n">
+        <x:v>0.01</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="I15" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:9">
+      <x:c r="A16" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="n">
+        <x:v>0.86</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:9">
+      <x:c r="A17" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="n">
+        <x:v>0.14</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I17" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:9">
+      <x:c r="A18" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="n">
+        <x:v>0.62</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="I18" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:9">
+      <x:c r="A19" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="n">
+        <x:v>0.47</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="I19" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:9">
+      <x:c r="A20" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="n">
+        <x:v>0.78</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G20" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="I20" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:9">
+      <x:c r="A21" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="n">
+        <x:v>0.88</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G21" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H21" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="I21" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:9">
+      <x:c r="A22" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="n">
+        <x:v>0.44</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="n">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F22" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G22" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="H22" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="I22" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>